<commit_message>
Work on filters in javafx
</commit_message>
<xml_diff>
--- a/UserSchedules.xlsx
+++ b/UserSchedules.xlsx
@@ -10,12 +10,12 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B357C4-4B25-4F36-94FF-38197E326293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="2" xr2:uid="{E7BA77D0-E1D3-4815-93D2-6EE54597C25D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="0" xr2:uid="{E7BA77D0-E1D3-4815-93D2-6EE54597C25D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kat" sheetId="3" r:id="rId1"/>
     <sheet name="Test2" sheetId="4" r:id="rId2"/>
-    <sheet name="testing" sheetId="5" r:id="rId4"/>
+    <sheet name="testing" r:id="rId8" sheetId="5"/>
+    <sheet name="Kat" r:id="rId9" sheetId="6"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>MATH 101</t>
   </si>
@@ -61,6 +61,42 @@
   </si>
   <si>
     <t>101</t>
+  </si>
+  <si>
+    <t>HUMA 202  A</t>
+  </si>
+  <si>
+    <t>CIV/LITERATURE</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>11:50:00</t>
+  </si>
+  <si>
+    <t>HAL</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>HUMA 302  A</t>
+  </si>
+  <si>
+    <t>MODERN CIV/INTL</t>
+  </si>
+  <si>
+    <t>MODERN CIV/INTL PERSP</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>12:50:00</t>
+  </si>
+  <si>
+    <t>304</t>
   </si>
 </sst>
 </file>
@@ -411,18 +447,6 @@
 </a:theme>
 </file>
 
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD3A52B8-E9D5-4339-B178-8C7A5427FF79}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953D2761-D321-4AA9-B437-78AABD2D384E}">
   <dimension ref="A1"/>
@@ -435,15 +459,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,6 +494,71 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>